<commit_message>
aggiunti fati oscillazioni smorzate
</commit_message>
<xml_diff>
--- a/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
+++ b/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
@@ -3,34 +3,135 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="oscillazioni libere" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="oscillazioni smorzate" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">omega (rad/s)</t>
+  </si>
+  <si>
+    <t>sigmaomega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essendo sigmaomega una sottostima dell'errore, assumiamo come incertezza su omega 0,01 rad/s</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega Medio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma omega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma omega zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma omega  misurazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma gamma misurazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev std omega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev std gamma</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega f</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="160" formatCode="0.0000"/>
+    <numFmt numFmtId="161" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -38,15 +139,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
+  <cellStyleXfs count="4">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="160" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="161" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,74 +515,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,7 +530,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -485,7 +556,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -574,7 +645,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -611,9 +682,385 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.421875"/>
+    <col bestFit="1" min="2" max="2" width="11.6640625"/>
+    <col customWidth="1" min="3" max="3" width="11.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.001</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.00089999999999999998</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.00089999999999999998</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.00080000000000000004</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>2.6200000000000001</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.00069999999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="3" max="3" width="23.76171875"/>
+    <col bestFit="1" min="4" max="4" width="23.8515625"/>
+    <col bestFit="1" min="5" max="5" width="16.421875"/>
+    <col bestFit="1" min="6" max="6" width="12.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="5">
+        <v>2.6600000000000001</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C2" s="7">
+        <f>AVERAGE(A2:A11)</f>
+        <v>2.7269999999999999</v>
+      </c>
+      <c r="D2" s="8">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.1744</v>
+      </c>
+      <c r="E2" s="9">
+        <f>SQRT(C2*C2+D2*D2)</f>
+        <v>2.7325710164605055</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="5">
+        <v>2.7400000000000002</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="5">
+        <v>2.7400000000000002</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="5">
+        <v>2.7200000000000002</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C5" s="7">
+        <f>SQRT(C8*C8+C10*C10)</f>
+        <v>0.068968591885485528</v>
+      </c>
+      <c r="D5" s="8">
+        <f>SQRT(D8*D8+D10*D10)</f>
+        <v>0.10021111049512758</v>
+      </c>
+      <c r="E5" s="9">
+        <f>(SQRT(POWER(2*C2*C5,2)+POWER(2*D2*D5,2)))/(2*SQRT(C2*C2+D2*D2))</f>
+        <v>0.069124501314900985</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="5">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="5">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.17000000000000001</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="5">
+        <v>2.7599999999999998</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.182</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.10000000000000001</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="5">
+        <v>2.7200000000000002</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.17999999999999999</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="5">
+        <v>2.7599999999999998</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C10" s="7">
+        <f>STDEV(A2:A11)</f>
+        <v>0.034009802508492455</v>
+      </c>
+      <c r="D10" s="8">
+        <f>STDEV(B2:B11)</f>
+        <v>0.0065012819248719388</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="5">
+        <v>2.77</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.187</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" s="5" t="e">
+        <f>2*PI()/A2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="5" t="e">
+        <f>2*PI()/A3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" s="5" t="e">
+        <f>2*PI()/A4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="5" t="e">
+        <f>2*PI()/A5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="5" t="e">
+        <f>2*PI()/A6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="5" t="e">
+        <f>2*PI()/A7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="5" t="e">
+        <f>2*PI()/A8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="5" t="e">
+        <f>2*PI()/A9</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="5" t="e">
+        <f>2*PI()/A10</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="5" t="e">
+        <f>2*PI()/A11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="5" t="e">
+        <f>2*PI()/A12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="5" t="e">
+        <f>2*PI()/A13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="5" t="e">
+        <f>2*PI()/A14</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="5" t="e">
+        <f>2*PI()/A15</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="5" t="e">
+        <f>2*PI()/A16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="5" t="e">
+        <f>2*PI()/A17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DATI PRIMA DI RIPRENDERE LE MISURE perchè è stato toccato il disco
</commit_message>
<xml_diff>
--- a/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
+++ b/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
@@ -65,7 +65,7 @@
     <t>T</t>
   </si>
   <si>
-    <t>A</t>
+    <t>M</t>
   </si>
   <si>
     <t xml:space="preserve">omega f</t>
@@ -161,8 +161,11 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -172,6 +175,7 @@
     <xf fontId="1" fillId="2" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="160" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="161" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,52 +704,113 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
         <v>2.6200000000000001</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0.001</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3">
         <v>2.6200000000000001</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0.00089999999999999998</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4">
         <v>2.6200000000000001</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.00089999999999999998</v>
       </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5">
         <v>2.6200000000000001</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>0.00080000000000000004</v>
       </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6">
         <v>2.6200000000000001</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.00069999999999999999</v>
       </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:L6"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -775,158 +840,158 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>2.6600000000000001</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>0.16900000000000001</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
         <f>AVERAGE(A2:A11)</f>
         <v>2.7269999999999999</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <f>AVERAGE(B2:B11)</f>
         <v>0.1744</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="10">
         <f>SQRT(C2*C2+D2*D2)</f>
         <v>2.7325710164605055</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>2.7400000000000002</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>0.17299999999999999</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>2.7400000000000002</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>0.17100000000000001</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>2.7200000000000002</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>0.16900000000000001</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <f>SQRT(C8*C8+C10*C10)</f>
         <v>0.068968591885485528</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <f>SQRT(D8*D8+D10*D10)</f>
         <v>0.10021111049512758</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="10">
         <f>(SQRT(POWER(2*C2*C5,2)+POWER(2*D2*D5,2)))/(2*SQRT(C2*C2+D2*D2))</f>
         <v>0.069124501314900985</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>2.7000000000000002</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>0.16800000000000001</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>2.7000000000000002</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>0.17000000000000001</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>2.7599999999999998</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>0.182</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>0.059999999999999998</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>0.10000000000000001</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>2.7200000000000002</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>0.17999999999999999</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>2.7599999999999998</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>0.17499999999999999</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <f>STDEV(A2:A11)</f>
         <v>0.034009802508492455</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <f>STDEV(B2:B11)</f>
         <v>0.0065012819248719388</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <v>2.77</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>0.187</v>
       </c>
     </row>
@@ -945,114 +1010,129 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2">
-      <c r="D2" s="5" t="e">
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="B2">
+        <v>3.1099999999999999</v>
+      </c>
+      <c r="C2" s="11">
+        <v>-0.062399999999999997</v>
+      </c>
+      <c r="D2">
+        <v>2.98</v>
+      </c>
+      <c r="E2" s="6">
         <f>2*PI()/A2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="D3" s="5" t="e">
+        <v>0.78149070984820734</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="E3" s="6" t="e">
         <f>2*PI()/A3</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4">
-      <c r="D4" s="5" t="e">
+    <row r="4" ht="14.25">
+      <c r="E4" s="6" t="e">
         <f>2*PI()/A4</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5">
-      <c r="D5" s="5" t="e">
+    <row r="5" ht="14.25">
+      <c r="E5" s="6" t="e">
         <f>2*PI()/A5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6">
-      <c r="D6" s="5" t="e">
+    <row r="6" ht="14.25">
+      <c r="E6" s="6" t="e">
         <f>2*PI()/A6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7">
-      <c r="D7" s="5" t="e">
+    <row r="7" ht="14.25">
+      <c r="E7" s="6" t="e">
         <f>2*PI()/A7</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8">
-      <c r="D8" s="5" t="e">
+    <row r="8" ht="14.25">
+      <c r="E8" s="6" t="e">
         <f>2*PI()/A8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9">
-      <c r="D9" s="5" t="e">
+    <row r="9" ht="14.25">
+      <c r="E9" s="6" t="e">
         <f>2*PI()/A9</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10">
-      <c r="D10" s="5" t="e">
+    <row r="10" ht="14.25">
+      <c r="E10" s="6" t="e">
         <f>2*PI()/A10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11">
-      <c r="D11" s="5" t="e">
+    <row r="11" ht="14.25">
+      <c r="E11" s="6" t="e">
         <f>2*PI()/A11</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12">
-      <c r="D12" s="5" t="e">
+    <row r="12" ht="14.25">
+      <c r="E12" s="6" t="e">
         <f>2*PI()/A12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13">
-      <c r="D13" s="5" t="e">
+    <row r="13" ht="14.25">
+      <c r="E13" s="6" t="e">
         <f>2*PI()/A13</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14">
-      <c r="D14" s="5" t="e">
+    <row r="14" ht="14.25">
+      <c r="E14" s="6" t="e">
         <f>2*PI()/A14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15">
-      <c r="D15" s="5" t="e">
+    <row r="15" ht="14.25">
+      <c r="E15" s="6" t="e">
         <f>2*PI()/A15</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16">
-      <c r="D16" s="5" t="e">
+    <row r="16" ht="14.25">
+      <c r="E16" s="6" t="e">
         <f>2*PI()/A16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17">
-      <c r="D17" s="5" t="e">
+    <row r="17" ht="14.25">
+      <c r="E17" s="6" t="e">
         <f>2*PI()/A17</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
raccolti faticosamente dati pendolo forzato non ne possiamo più
</commit_message>
<xml_diff>
--- a/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
+++ b/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="oscillazioni libere" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">omega (rad/s)</t>
   </si>
@@ -65,10 +65,13 @@
     <t>T</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">omega f</t>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>omegaf</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,6 +186,8 @@
     <xf fontId="3" fillId="4" borderId="0" numFmtId="161" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,115 +1028,234 @@
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="C2" s="12"/>
-      <c r="E2" s="6" t="e">
+      <c r="A2" s="6">
+        <v>4.3200000000000003</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.45</v>
+      </c>
+      <c r="E2" s="6">
         <f>2*PI()/A2</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>1.4544410433286079</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="E3" s="6" t="e">
-        <f>2*PI()/A3</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A3" s="6">
+        <v>3.9100000000000001</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1.8999999999999999</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.9500000000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.6100000000000001</v>
+      </c>
+      <c r="E3" s="6">
+        <f>6.28/A3</f>
+        <v>1.6061381074168799</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="E4" s="6" t="e">
+      <c r="A4" s="6">
+        <v>3.5499999999999998</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.4300000000000002</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="E4" s="6">
         <f>2*PI()/A4</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>1.7699113541350948</v>
+      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="E5" s="6" t="e">
+      <c r="A5" s="6">
+        <v>3.04</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.1499999999999999</v>
+      </c>
+      <c r="E5" s="6">
         <f>2*PI()/A5</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>2.0668372720985482</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="E6" s="6" t="e">
-        <f>2*PI()/A6</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A6" s="6">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2.3999999999999999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E6" s="6">
+        <f>6.28/A6</f>
+        <v>2.4627450980392158</v>
+      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="E7" s="6" t="e">
+      <c r="A7" s="6">
+        <v>2.3999999999999999</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="6">
+        <v>11.800000000000001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2.6600000000000001</v>
+      </c>
+      <c r="E7" s="6">
         <f>2*PI()/A7</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>2.6179938779914944</v>
+      </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="E8" s="6" t="e">
+      <c r="A8" s="6">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="C8" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2.79</v>
+      </c>
+      <c r="E8" s="6">
         <f>2*PI()/A8</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>2.780170489902472</v>
+      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="E9" s="6" t="e">
+      <c r="A9" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="C9" s="6">
+        <v>6.2800000000000002</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2.8599999999999999</v>
+      </c>
+      <c r="E9" s="6">
         <f>2*PI()/A9</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>2.8821950950365074</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="E10" s="6" t="e">
+      <c r="A10" s="6">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2.7999999999999998</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3.0600000000000001</v>
+      </c>
+      <c r="E10" s="6">
         <f>2*PI()/A10</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>3.0353552208597039</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="E11" s="6" t="e">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2.8999999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3.75</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3.1400000000000001</v>
+      </c>
+      <c r="E11" s="14">
         <f>2*PI()/A11</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="E12" s="6" t="e">
-        <f>2*PI()/A12</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="E13" s="6" t="e">
-        <f>2*PI()/A13</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="E14" s="6" t="e">
-        <f>2*PI()/A14</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="E15" s="6" t="e">
-        <f>2*PI()/A15</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="E16" s="6" t="e">
-        <f>2*PI()/A16</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="E17" s="6" t="e">
-        <f>2*PI()/A17</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="F18" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
plot oscillazioni smorzate forzate
</commit_message>
<xml_diff>
--- a/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
+++ b/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
@@ -8,7 +8,7 @@
   <sheets>
     <sheet name="oscillazioni libere" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="oscillazioni smorzate" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="oscillazioni forzate" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -170,7 +170,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,8 +186,6 @@
     <xf fontId="3" fillId="4" borderId="0" numFmtId="161" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,7 +1032,7 @@
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1043,58 +1041,58 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="6">
-        <v>4.3200000000000003</v>
+        <v>3.9100000000000001</v>
       </c>
       <c r="B2" s="6">
-        <v>1.78</v>
+        <v>1.8999999999999999</v>
       </c>
       <c r="C2" s="6">
-        <v>2.4500000000000002</v>
+        <v>2.9500000000000002</v>
       </c>
       <c r="D2" s="6">
-        <v>1.45</v>
+        <v>1.6100000000000001</v>
       </c>
       <c r="E2" s="6">
-        <f>2*PI()/A2</f>
-        <v>1.4544410433286079</v>
+        <f>6.28/A2</f>
+        <v>1.6061381074168799</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="6">
-        <v>3.9100000000000001</v>
+        <v>3.5499999999999998</v>
       </c>
       <c r="B3" s="6">
-        <v>1.8999999999999999</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>2.9500000000000002</v>
+        <v>3.4300000000000002</v>
       </c>
       <c r="D3" s="6">
-        <v>1.6100000000000001</v>
+        <v>1.78</v>
       </c>
       <c r="E3" s="6">
-        <f>6.28/A3</f>
-        <v>1.6061381074168799</v>
+        <f t="shared" ref="E3:E7" si="0">2*PI()/A3</f>
+        <v>1.7699113541350948</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="6">
-        <v>3.5499999999999998</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="B4" s="6">
-        <v>2</v>
+        <v>2.1000000000000001</v>
       </c>
       <c r="C4" s="6">
-        <v>3.4300000000000002</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D4" s="6">
-        <v>1.78</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E4" s="6">
-        <f>2*PI()/A4</f>
-        <v>1.7699113541350948</v>
+        <f t="shared" si="0"/>
+        <v>1.9634954084936207</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -1112,150 +1110,253 @@
         <v>2.1499999999999999</v>
       </c>
       <c r="E5" s="6">
-        <f>2*PI()/A5</f>
+        <f t="shared" si="0"/>
         <v>2.0668372720985482</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="6">
-        <v>2.5499999999999998</v>
+        <v>2.79</v>
       </c>
       <c r="B6" s="6">
-        <v>2.3999999999999999</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C6" s="6">
-        <v>12.4</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="D6" s="6">
-        <v>2.4500000000000002</v>
+        <v>2.23</v>
       </c>
       <c r="E6" s="6">
-        <f>6.28/A6</f>
-        <v>2.4627450980392158</v>
+        <f t="shared" si="0"/>
+        <v>2.2520377445088124</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="6">
-        <v>2.3999999999999999</v>
+        <v>2.6600000000000001</v>
       </c>
       <c r="B7" s="6">
-        <v>2.5</v>
+        <v>2.3500000000000001</v>
       </c>
       <c r="C7" s="6">
-        <v>11.800000000000001</v>
+        <v>9.3900000000000006</v>
       </c>
       <c r="D7" s="6">
-        <v>2.6600000000000001</v>
+        <v>2.3700000000000001</v>
       </c>
       <c r="E7" s="6">
-        <f>2*PI()/A7</f>
-        <v>2.6179938779914944</v>
+        <f t="shared" si="0"/>
+        <v>2.3620997395411978</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="6">
-        <v>2.2599999999999998</v>
+        <v>2.54</v>
       </c>
       <c r="B8" s="6">
-        <v>2.6000000000000001</v>
+        <v>2.3999999999999999</v>
       </c>
       <c r="C8" s="6">
-        <v>10.5</v>
+        <v>11.9</v>
       </c>
       <c r="D8" s="6">
-        <v>2.79</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="E8" s="6">
-        <f>2*PI()/A8</f>
-        <v>2.780170489902472</v>
+        <f>6.28/A8</f>
+        <v>2.4724409448818898</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="6">
-        <v>2.1800000000000002</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="B9" s="6">
-        <v>2.7000000000000002</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="C9" s="6">
-        <v>6.2800000000000002</v>
+        <v>11.800000000000001</v>
       </c>
       <c r="D9" s="6">
-        <v>2.8599999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="E9" s="6">
         <f>2*PI()/A9</f>
-        <v>2.8821950950365074</v>
+        <v>2.5233675932448136</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="6">
-        <v>2.0699999999999998</v>
+        <v>2.3999999999999999</v>
       </c>
       <c r="B10" s="6">
-        <v>2.7999999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="C10" s="6">
-        <v>4.8499999999999996</v>
+        <v>11.800000000000001</v>
       </c>
       <c r="D10" s="6">
-        <v>3.0600000000000001</v>
+        <v>2.6600000000000001</v>
       </c>
       <c r="E10" s="6">
-        <f>2*PI()/A10</f>
-        <v>3.0353552208597039</v>
+        <f t="shared" ref="E10:E15" si="1">2*PI()/A10</f>
+        <v>2.6179938779914944</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="6">
+        <v>2.3500000000000001</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2.6000000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2.71</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6736958753955684</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="6">
+        <v>2.3100000000000001</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2.6499999999999999</v>
+      </c>
+      <c r="C12" s="6">
+        <v>9.9800000000000004</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2.73</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7199936394716824</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6.2800000000000002</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.8599999999999999</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8821950950365074</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="6">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2.7999999999999998</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D14" s="6">
+        <v>3.0600000000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0353552208597039</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B15" s="6">
         <v>2.8999999999999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C15" s="6">
         <v>3.75</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D15" s="6">
         <v>3.1400000000000001</v>
       </c>
-      <c r="E11" s="14">
-        <f>2*PI()/A11</f>
+      <c r="E15" s="6">
+        <f t="shared" si="1"/>
         <v>3.1415926535897931</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" ht="14.25">
       <c r="F15" s="6"/>
     </row>
     <row r="16" ht="14.25">
+      <c r="A16" s="6">
+        <v>1.9199999999999999</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="6">
+        <v>3.29</v>
+      </c>
+      <c r="E16" s="6">
+        <f>2*PI()/A16</f>
+        <v>3.2724923474893681</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" ht="14.25">
+      <c r="A17" s="6">
+        <v>1.8100000000000001</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3.1000000000000001</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2.8999999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3.5499999999999998</v>
+      </c>
+      <c r="E17" s="6">
+        <f>2*PI()/A17</f>
+        <v>3.4713730978892738</v>
+      </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" ht="14.25">
       <c r="F18" s="6"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="F22" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
oscillazioni forzate smorzate rivisto
</commit_message>
<xml_diff>
--- a/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
+++ b/OSCILLAZIONI FORZATE SMORZATE/oscillazioni_forzate_smorzate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="oscillazioni libere" sheetId="1" state="visible" r:id="rId1"/>
@@ -880,6 +880,7 @@
         <v>2.5762062592114017</v>
       </c>
       <c r="F2" s="2"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="6">
@@ -918,15 +919,15 @@
       </c>
       <c r="C5" s="11">
         <f>SQRT(C8*C8+C10*C10)</f>
-        <v>0.069992063042097027</v>
+        <v>0.037401723073795481</v>
       </c>
       <c r="D5" s="9">
         <f>SQRT(D8*D8+D10*D10)</f>
-        <v>0.10024752698529112</v>
+        <v>0.0071110243050257291</v>
       </c>
       <c r="E5" s="10">
         <f>(SQRT(POWER(2*C2*C5,2)+POWER(2*D2*D5,2)))/(2*SQRT(C2*C2+D2*D2))</f>
-        <v>0.070140472472493123</v>
+        <v>0.037328872773883637</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -961,10 +962,10 @@
         <v>0.158</v>
       </c>
       <c r="C8" s="3">
-        <v>0.059999999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="D8" s="4">
-        <v>0.10000000000000001</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="9" ht="14.25">
@@ -1205,7 +1206,7 @@
         <v>2.6600000000000001</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" ref="E10:E15" si="1">2*PI()/A10</f>
+        <f t="shared" ref="E10:E17" si="1">2*PI()/A10</f>
         <v>2.6179938779914944</v>
       </c>
       <c r="F10" s="6"/>
@@ -1319,7 +1320,7 @@
         <v>3.29</v>
       </c>
       <c r="E16" s="6">
-        <f>2*PI()/A16</f>
+        <f t="shared" si="1"/>
         <v>3.2724923474893681</v>
       </c>
       <c r="F16" s="6"/>
@@ -1338,7 +1339,7 @@
         <v>3.5499999999999998</v>
       </c>
       <c r="E17" s="6">
-        <f>2*PI()/A17</f>
+        <f t="shared" si="1"/>
         <v>3.4713730978892738</v>
       </c>
       <c r="F17" s="6"/>

</xml_diff>